<commit_message>
mis à jour to do
</commit_message>
<xml_diff>
--- a/todo_avancement.xlsx
+++ b/todo_avancement.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s.rakotoarison\Documents\ITU-semestre-7\Rojo\project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s.rakotoarison\Documents\ITU-semestre-7\Rojo\git\m1p9mean-danih\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="23040" windowHeight="9180"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="23040" windowHeight="9180"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -419,8 +419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -491,20 +491,23 @@
         <v>30</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F6">
         <f>D6-E6</f>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <f>(E6*100%)/D6</f>
-        <v>0</v>
+        <f>((E6*100%)/D6)*100</f>
+        <v>100</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J6" s="2"/>
+      <c r="J6" s="2">
+        <f>SUM(D6:D9)</f>
+        <v>220</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -520,20 +523,23 @@
         <v>10</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F7">
         <f t="shared" ref="F7:F9" si="0">D7-E7</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <f t="shared" ref="G7:G9" si="1">(E7*100%)/D7</f>
-        <v>0</v>
+        <f t="shared" ref="G7:G9" si="1">((E7*100%)/D7)*100</f>
+        <v>100</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J7" s="2"/>
+      <c r="J7" s="2">
+        <f>SUM(E6:E9)</f>
+        <v>220</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -549,20 +555,23 @@
         <v>60</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="G8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J8" s="2"/>
+      <c r="J8" s="2">
+        <f>J6-J7</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -578,15 +587,15 @@
         <v>120</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="G9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>